<commit_message>
Includes Dialog box for search
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F236F399-A3EE-49FB-87A6-2D3250826C1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4EBA3A-5CE5-4A14-87B5-179EF2EA9C3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="16645" windowHeight="6120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{C07F8D51-F8E9-4EFF-B858-A97A0488BD97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Title</t>
   </si>
@@ -36,72 +36,24 @@
     <t>Agency</t>
   </si>
   <si>
-    <t>Supply, delivery, installation, testing and commissioning of Electronic Key Management System (EKMS) for School of Engineering</t>
+    <t>Book Vouchers for Honours Day 2021</t>
+  </si>
+  <si>
+    <t>05 May 2021
+01:00PM</t>
+  </si>
+  <si>
+    <t>Ministry of Education - Schools</t>
+  </si>
+  <si>
+    <t>PROCUREMENT BOOK VOUCHERS FOR SINGAPORE SCIENCE AND ENGINEERING FAIR 2021</t>
   </si>
   <si>
     <t>06 May 2021
 01:00PM</t>
   </si>
   <si>
-    <t>Nanyang Polytechnic</t>
-  </si>
-  <si>
-    <t>ITQ FOR PERSONAL PROTECTION EQUIPMENT FOR USE ON ADVENTURE LEARNING FACILITIES</t>
-  </si>
-  <si>
-    <t>Ministry of Education</t>
-  </si>
-  <si>
-    <t>Primary 4 APEX Leadership Fiesta 2021</t>
-  </si>
-  <si>
-    <t>Ministry of Education - Schools</t>
-  </si>
-  <si>
-    <t>Provision of Group Term Life Insurance Coverage for a period of 2 years with an option to extend for another 1 year</t>
-  </si>
-  <si>
-    <t>Accounting And Corporate Regulatory Authority</t>
-  </si>
-  <si>
-    <t>INVITATION TO QUOTE FOR ENGAGEMENT OF MALAY LANGUAGE RESOURCE PERSON FOR REVIEW OF MOE KINDERGARTEN (MK) CURRICULUM RESOURCES</t>
-  </si>
-  <si>
-    <t>11 May 2021
-01:00PM</t>
-  </si>
-  <si>
-    <t>Provision of Medical Services</t>
-  </si>
-  <si>
-    <t>20 May 2021
-04:00PM</t>
-  </si>
-  <si>
-    <t>Ministry of Home Affairs - Ministry Headquarter 1</t>
-  </si>
-  <si>
-    <t>PERIOD CONTRACT FOR THE SUPPLY AND DELIVERY OF CHEMICALS AND CONSUMABLES FOR 12 MONTHS</t>
-  </si>
-  <si>
-    <t>27 May 2021
-04:00PM</t>
-  </si>
-  <si>
-    <t>INVITATION TO TENDER FOR THE SUPPLY, DELIVERY, SUPPORT OF ORACLE DATABASE AND MIDDLEWARE LICENCE AND SUPPORT RENEWAL</t>
-  </si>
-  <si>
-    <t>24 May 2021
-04:00PM</t>
-  </si>
-  <si>
-    <t>Ministry of Social and Family Development - Ministry Headquarter</t>
-  </si>
-  <si>
-    <t>PROVISION OF STANDARD FIRST AID CERTIFICATION COURSE WITH BLENDED LEARNING FOR STAFF OF GREENWOOD PRIMARY SCHOOL</t>
-  </si>
-  <si>
-    <t>ITQ for the supply, delivery, installation, testing and commissioning of laboratory washer</t>
+    <t>Science Centre Board</t>
   </si>
 </sst>
 </file>
@@ -176,7 +128,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -188,7 +140,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -235,6 +187,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -270,6 +239,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,16 +407,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EC72ED-9BC1-4067-A293-083897307D1E}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="128.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.04296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.75">
@@ -444,114 +430,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="36.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Includes both Data Scrapping for Quotation and the rest of the portion (in 2 DataTables)
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4EBA3A-5CE5-4A14-87B5-179EF2EA9C3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1979F92E-61A5-46C9-93DC-AFDC7AF79011}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{C07F8D51-F8E9-4EFF-B858-A97A0488BD97}"/>
+    <workbookView xWindow="440" yWindow="45" windowWidth="14010" windowHeight="5585" xr2:uid="{C07F8D51-F8E9-4EFF-B858-A97A0488BD97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,35 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Title</t>
+    <t>Quotation</t>
   </si>
   <si>
-    <t>Closing On</t>
+    <t>Quotation - MOESCHETQ21002160</t>
   </si>
   <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>Book Vouchers for Honours Day 2021</t>
-  </si>
-  <si>
-    <t>05 May 2021
-01:00PM</t>
-  </si>
-  <si>
-    <t>Ministry of Education - Schools</t>
-  </si>
-  <si>
-    <t>PROCUREMENT BOOK VOUCHERS FOR SINGAPORE SCIENCE AND ENGINEERING FAIR 2021</t>
-  </si>
-  <si>
-    <t>06 May 2021
-01:00PM</t>
-  </si>
-  <si>
-    <t>Science Centre Board</t>
+    <t>Quotation - SCB000ETQ21000015</t>
   </si>
 </sst>
 </file>
@@ -89,11 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +385,8 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EC72ED-9BC1-4067-A293-083897307D1E}">
-  <dimension ref="A1:C3"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,37 +397,19 @@
     <col min="3" max="3" width="25.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
With each Quotaton id
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EBF5EF-B620-434D-BF0A-5537891BAE71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104C64FF-E131-43E6-AB2D-6C719BEDB7B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{A22D2129-1FA2-47FD-99A5-AE5E5C814005}"/>
+    <workbookView xWindow="2675" yWindow="4615" windowWidth="14010" windowHeight="5585" xr2:uid="{DA6E02D8-13E9-4AA3-870B-6EC15A9D3B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBBA129-FDA0-4FF4-BECB-B610A70E6EC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65F8DE-3029-4B9F-899E-DACB20885E8C}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Enhancements to pull the 3rd (most recent) voucher item
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E644AFB-2261-40D6-9FE1-7000042728EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E65626-6601-4203-90E5-5A60EB378B40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2675" yWindow="4615" windowWidth="14010" windowHeight="5585" xr2:uid="{DA6E02D8-13E9-4AA3-870B-6EC15A9D3B31}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Quotation</t>
   </si>
@@ -69,6 +69,19 @@
   </si>
   <si>
     <t>Science Centre Board</t>
+  </si>
+  <si>
+    <t>Quotation - MOE000ETQ21000131</t>
+  </si>
+  <si>
+    <t>INVITATION TO QUOTE FOR BOOK VOUCHERS</t>
+  </si>
+  <si>
+    <t>19 May 2021
+01:00PM</t>
+  </si>
+  <si>
+    <t>Ministry of Education</t>
   </si>
 </sst>
 </file>
@@ -424,11 +437,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65F8DE-3029-4B9F-899E-DACB20885E8C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.04296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.40625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -449,16 +471,16 @@
     </row>
     <row r="2" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -466,18 +488,35 @@
     </row>
     <row r="3" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set AlterIfDisabled = True for 'Download All' button
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E65626-6601-4203-90E5-5A60EB378B40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06919621-228A-4468-8DEA-9050A9241D68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2675" yWindow="4615" windowWidth="14010" windowHeight="5585" xr2:uid="{DA6E02D8-13E9-4AA3-870B-6EC15A9D3B31}"/>
+    <workbookView xWindow="2675" yWindow="4615" windowWidth="14010" windowHeight="5585" xr2:uid="{282DFD42-2C25-4C53-9D03-BE56E9A2FC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,22 @@
     <t>Procurement Category</t>
   </si>
   <si>
+    <t>Quotation - MOE000ETQ21000131</t>
+  </si>
+  <si>
+    <t>INVITATION TO QUOTE FOR BOOK VOUCHERS</t>
+  </si>
+  <si>
+    <t>19 May 2021
+01:00PM</t>
+  </si>
+  <si>
+    <t>Ministry of Education</t>
+  </si>
+  <si>
+    <t>Administration &amp; Training ⇒ Gifts &amp; Souvenirs</t>
+  </si>
+  <si>
     <t>Quotation - MOESCHETQ21002160</t>
   </si>
   <si>
@@ -55,9 +71,6 @@
     <t>Ministry of Education - Schools</t>
   </si>
   <si>
-    <t>Administration &amp; Training ⇒ Gifts &amp; Souvenirs</t>
-  </si>
-  <si>
     <t>Quotation - SCB000ETQ21000015</t>
   </si>
   <si>
@@ -69,19 +82,6 @@
   </si>
   <si>
     <t>Science Centre Board</t>
-  </si>
-  <si>
-    <t>Quotation - MOE000ETQ21000131</t>
-  </si>
-  <si>
-    <t>INVITATION TO QUOTE FOR BOOK VOUCHERS</t>
-  </si>
-  <si>
-    <t>19 May 2021
-01:00PM</t>
-  </si>
-  <si>
-    <t>Ministry of Education</t>
   </si>
 </sst>
 </file>
@@ -435,13 +435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65F8DE-3029-4B9F-899E-DACB20885E8C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA340546-5E4F-4606-A4B6-4A5621805954}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -471,16 +469,16 @@
     </row>
     <row r="2" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -488,16 +486,16 @@
     </row>
     <row r="3" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -505,16 +503,16 @@
     </row>
     <row r="4" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
With select folder box
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38FE744-DC69-4D02-B232-A7EA06BBF655}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143D9E3-A000-4C56-B6C8-B789B73724EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2675" yWindow="4615" windowWidth="14010" windowHeight="5585" xr2:uid="{282DFD42-2C25-4C53-9D03-BE56E9A2FC01}"/>
+    <workbookView xWindow="2060" yWindow="2435" windowWidth="16540" windowHeight="7765" xr2:uid="{282DFD42-2C25-4C53-9D03-BE56E9A2FC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Quotation</t>
   </si>
@@ -56,32 +56,6 @@
   </si>
   <si>
     <t>Administration &amp; Training ⇒ Gifts &amp; Souvenirs</t>
-  </si>
-  <si>
-    <t>Quotation - MOESCHETQ21002160</t>
-  </si>
-  <si>
-    <t>Book Vouchers for Honours Day 2021</t>
-  </si>
-  <si>
-    <t>05 May 2021
-01:00PM</t>
-  </si>
-  <si>
-    <t>Ministry of Education - Schools</t>
-  </si>
-  <si>
-    <t>Quotation - SCB000ETQ21000015</t>
-  </si>
-  <si>
-    <t>PROCUREMENT BOOK VOUCHERS FOR SINGAPORE SCIENCE AND ENGINEERING FAIR 2021</t>
-  </si>
-  <si>
-    <t>06 May 2021
-01:00PM</t>
-  </si>
-  <si>
-    <t>Science Centre Board</t>
   </si>
 </sst>
 </file>
@@ -437,17 +411,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA340546-5E4F-4606-A4B6-4A5621805954}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.04296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.40625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
@@ -484,40 +461,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Include links for each pdf doc
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D253BF-B71E-464F-BC9F-744911ED533C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6623EDE-563B-4E4A-B3D0-D4FB5D5D9476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="2435" windowWidth="16540" windowHeight="7765" xr2:uid="{282DFD42-2C25-4C53-9D03-BE56E9A2FC01}"/>
+    <workbookView xWindow="200" yWindow="0" windowWidth="12140" windowHeight="7765" xr2:uid="{8221A3C1-6818-4C6A-96E7-11B85E9BA2DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Quotation</t>
   </si>
@@ -40,32 +40,59 @@
   </si>
   <si>
     <t>Procurement Category</t>
-  </si>
-  <si>
-    <t>Quotation - MOE000ETQ21000131</t>
-  </si>
-  <si>
-    <t>INVITATION TO QUOTE FOR BOOK VOUCHERS</t>
   </si>
   <si>
     <t>19 May 2021
 01:00PM</t>
   </si>
   <si>
-    <t>Ministry of Education</t>
-  </si>
-  <si>
-    <t>Administration &amp; Training ⇒ Gifts &amp; Souvenirs</t>
+    <t>Quotation - MOESCHETQ21002323</t>
+  </si>
+  <si>
+    <t>Supply of Instructor for Basketball Girls CCA Training Programme</t>
+  </si>
+  <si>
+    <t>Ministry of Education - Schools</t>
+  </si>
+  <si>
+    <t>Services ⇒ Data Entry, Supply of Manpower Services</t>
+  </si>
+  <si>
+    <t>Quotation - MOESCHETQ21002298</t>
+  </si>
+  <si>
+    <t>Provision of Coaching Services for Basketball (Girls) CCA</t>
+  </si>
+  <si>
+    <t>12 May 2021
+01:00PM</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>N:\Temp2\MOESCHETQ21002323\MOESCHETQ21002323.zip</t>
+  </si>
+  <si>
+    <t>N:\Temp2\MOESCHETQ21002298\MOESCHETQ21002298.zip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,16 +115,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,25 +439,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA340546-5E4F-4606-A4B6-4A5621805954}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93D3E15-9CF7-4A8D-A988-F726F0405F76}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.6796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,16 +473,19 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -460,8 +493,35 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{D64B5B84-EA42-43BD-8B18-194059A34C14}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{E3A5EFCA-D7CD-4C99-8F1C-8B106A9B15A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhancement on the "Type into" selector for the search box in Gebiz
</commit_message>
<xml_diff>
--- a/Data/Output.xlsx
+++ b/Data/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAC01_TrackingOfTenders\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6623EDE-563B-4E4A-B3D0-D4FB5D5D9476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE58BD1C-C6AB-49B5-AC4B-70493344A1EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="0" windowWidth="12140" windowHeight="7765" xr2:uid="{8221A3C1-6818-4C6A-96E7-11B85E9BA2DC}"/>
+    <workbookView xWindow="1075" yWindow="2795" windowWidth="17055" windowHeight="5235" xr2:uid="{8221A3C1-6818-4C6A-96E7-11B85E9BA2DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -519,8 +519,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{D64B5B84-EA42-43BD-8B18-194059A34C14}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{E3A5EFCA-D7CD-4C99-8F1C-8B106A9B15A9}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{18FB7E2C-4615-49F2-8FEA-F125A7CC1270}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{A8E4A1CD-CF1A-4BF6-A6F7-0D5D2769A9E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>